<commit_message>
implement view game result
</commit_message>
<xml_diff>
--- a/datafiles/player.xlsx
+++ b/datafiles/player.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="76">
   <si>
     <t>Position</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -255,6 +255,70 @@
   </si>
   <si>
     <t>Cote dIvoire</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Steven Gerrard</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Coutinho</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Jordan Henderson</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Adam Lallana</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lucas</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Emre Can</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Joe Allen</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Suso</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Raheem Sterling</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lazar Marković</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Serbia</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rickie Lambert</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Daniel Sturridge</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fabio Borini</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Italy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mario Balotelli</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -616,10 +680,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G33"/>
+  <dimension ref="A1:G47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
+      <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -1389,6 +1453,328 @@
       </c>
       <c r="G33" s="2">
         <v>181</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C34" s="2">
+        <v>34</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E34" s="2">
+        <v>8</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G34" s="2">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C35" s="2">
+        <v>2</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E35" s="2">
+        <v>10</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G35" s="2">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C36" s="2">
+        <v>24</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E36" s="2">
+        <v>14</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G36" s="2">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C37" s="2">
+        <v>26</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E37" s="2">
+        <v>20</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G37" s="2">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C38" s="2">
+        <v>27</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E38" s="2">
+        <v>21</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G38" s="2">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C39" s="2">
+        <v>23</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E39" s="2">
+        <v>23</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G39" s="2">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="A40" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C40" s="2">
+        <v>24</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E40" s="2">
+        <v>24</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G40" s="2">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C41" s="2">
+        <v>20</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E41" s="2">
+        <v>30</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G41" s="2">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
+      <c r="A42" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C42" s="2">
+        <v>19</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E42" s="2">
+        <v>31</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G42" s="2">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
+      <c r="A43" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C43" s="2">
+        <v>20</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E43" s="2">
+        <v>50</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G43" s="2">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="A44" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C44" s="2">
+        <v>32</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E44" s="2">
+        <v>9</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G44" s="2">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
+      <c r="A45" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C45" s="2">
+        <v>25</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E45" s="2">
+        <v>15</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G45" s="2">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
+      <c r="A46" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C46" s="2">
+        <v>23</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E46" s="2">
+        <v>29</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G46" s="2">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
+      <c r="A47" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C47" s="2">
+        <v>24</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E47" s="2">
+        <v>45</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G47" s="2">
+        <v>189</v>
       </c>
     </row>
   </sheetData>

</xml_diff>